<commit_message>
PDF REPORTS AND SMS
</commit_message>
<xml_diff>
--- a/required/templates/ofptemplate-temp.xlsx
+++ b/required/templates/ofptemplate-temp.xlsx
@@ -44,9 +44,6 @@
     <t>ORDER OF PAYMENT</t>
   </si>
   <si>
-    <t>Control No. ________________</t>
-  </si>
-  <si>
     <t>IN :</t>
   </si>
   <si>
@@ -192,12 +189,15 @@
   <si>
     <t>, as follows</t>
   </si>
+  <si>
+    <t>Control No.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +262,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -410,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -427,6 +436,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -472,6 +484,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -502,6 +520,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -514,16 +535,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -911,95 +925,107 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
     <col min="10" max="10" width="6.140625" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="Q2" s="21" t="s">
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="Q3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+    </row>
+    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="H4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+    </row>
+    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="H5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="H6" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="H7" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="R7" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-    </row>
-    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="H4" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-    </row>
-    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="H5" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-    </row>
-    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="H6" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-    </row>
-    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="H7" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="R7" s="41" t="s">
+      <c r="S7" s="45"/>
+    </row>
+    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G8" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="R8" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="41"/>
-    </row>
-    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G8" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="R8" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="S8" s="41"/>
+      <c r="S8" s="45"/>
     </row>
     <row r="10" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="12" spans="4:20" x14ac:dyDescent="0.25">
       <c r="Q12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R12" s="13"/>
       <c r="S12" s="1"/>
@@ -1007,23 +1033,23 @@
     </row>
     <row r="15" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="F15" s="43"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="K15" s="12"/>
       <c r="L15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1035,15 +1061,15 @@
     </row>
     <row r="16" spans="4:20" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
       <c r="K16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1053,204 +1079,204 @@
       <c r="Q16" s="1"/>
     </row>
     <row r="19" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37" t="s">
+      <c r="H19" s="40"/>
+      <c r="I19" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37" t="s">
+      <c r="J19" s="40"/>
+      <c r="K19" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37" t="s">
+      <c r="L19" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="L19" s="37" t="s">
+      <c r="O19" s="40"/>
+      <c r="P19" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37" t="s">
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37" t="s">
+      <c r="S19" s="40"/>
+    </row>
+    <row r="20" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+    </row>
+    <row r="21" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="31"/>
+    </row>
+    <row r="22" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="33"/>
+    </row>
+    <row r="23" spans="5:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E23" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="S19" s="37"/>
-    </row>
-    <row r="20" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-    </row>
-    <row r="21" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="44"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="44"/>
-    </row>
-    <row r="22" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="30"/>
-    </row>
-    <row r="23" spans="5:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E23" s="34" t="s">
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="31"/>
+    </row>
+    <row r="24" spans="5:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="31"/>
+    </row>
+    <row r="25" spans="5:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="44"/>
-    </row>
-    <row r="24" spans="5:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="27" t="s">
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="44"/>
-    </row>
-    <row r="25" spans="5:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="44"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="31"/>
     </row>
     <row r="28" spans="5:19" x14ac:dyDescent="0.25">
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
     <row r="30" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="K30" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="L30" s="22"/>
+    </row>
+    <row r="31" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="G31" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="K30" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="L30" s="21"/>
-    </row>
-    <row r="31" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="G31" s="21" t="s">
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="L31" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="L31" s="21" t="s">
+      <c r="M31" s="22"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+    </row>
+    <row r="35" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E35" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-    </row>
-    <row r="35" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E35" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="18"/>
     </row>
     <row r="36" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E36" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -1270,16 +1296,16 @@
     <row r="37" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E37" s="7"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
+      <c r="G37" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -1291,20 +1317,20 @@
     <row r="38" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E38" s="7"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
+      <c r="G38" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
-      <c r="M38" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
+      <c r="M38" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
       <c r="S38" s="6"/>
@@ -1329,18 +1355,18 @@
     <row r="40" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E40" s="7"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
+      <c r="G40" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="6"/>
@@ -1351,11 +1377,11 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
+      <c r="J41" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
@@ -1382,10 +1408,10 @@
       <c r="S42" s="6"/>
     </row>
     <row r="43" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E43" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F43" s="14"/>
+      <c r="E43" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="15"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -1403,17 +1429,17 @@
     <row r="44" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E44" s="7"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
+      <c r="G44" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
@@ -1424,17 +1450,17 @@
     <row r="45" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E45" s="7"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
+      <c r="G45" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
@@ -1445,17 +1471,17 @@
     <row r="46" spans="5:19" x14ac:dyDescent="0.25">
       <c r="E46" s="7"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="14" t="s">
+      <c r="G46" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
@@ -1482,17 +1508,17 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R2:S4"/>
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="H5:L5"/>
     <mergeCell ref="H6:L6"/>
     <mergeCell ref="H7:L7"/>
     <mergeCell ref="G8:M8"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R8:S8"/>
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="N19:O20"/>
     <mergeCell ref="P19:Q20"/>

</xml_diff>